<commit_message>
updates to send just one email
</commit_message>
<xml_diff>
--- a/subscriptions.xlsx
+++ b/subscriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hashmilhan/Developer/subscription-notification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E15CF5C-1C9F-304D-8BB3-AE49B7BFE0B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7D24A56-CCCD-664E-8996-8A34A405FB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{178403A2-B36F-A743-9837-73DB81AA4E7D}"/>
   </bookViews>
@@ -409,7 +409,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -427,7 +427,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>44965</v>
+        <v>44993</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -435,7 +435,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>44972</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -443,7 +443,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>44973</v>
+        <v>45001</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -451,7 +451,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>44972</v>
+        <v>45000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>